<commit_message>
Cleaned up lab and field wings
Made better wing source files for future analysis of field and lab, excluded all trace of tpn 7
</commit_message>
<xml_diff>
--- a/MorphoJ shape field and lab/2017_10_15 Morphoj Field 18 results cva pca.xlsx
+++ b/MorphoJ shape field and lab/2017_10_15 Morphoj Field 18 results cva pca.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\virgc\GitHub\wingproj\MorphoJ shape field and lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vmc04\Documents\GitHub\wingproj\MorphoJ shape field and lab\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="10410" activeTab="3" xr2:uid="{39FE9C61-65AD-4D66-8830-3064A8F4A832}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18270" windowHeight="10410"/>
   </bookViews>
   <sheets>
     <sheet name="Data table field" sheetId="1" r:id="rId1"/>
@@ -173,7 +173,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -465,15 +465,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -487,6 +478,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -499,10 +503,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1031,11 +1031,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A205BAB-A834-4FC8-8917-BEF9D4D21D23}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:S31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1067,7 @@
       </c>
     </row>
     <row r="6" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="21" t="s">
         <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1083,13 +1083,13 @@
         <f>O11 &amp; " " &amp;$M$12&amp; " " &amp; R11</f>
         <v>2.92 ± 0.2</v>
       </c>
-      <c r="G6" s="17" t="str">
+      <c r="G6" s="14" t="str">
         <f>P11 &amp; " " &amp;$M$12&amp; " " &amp; S11</f>
         <v>2.7 ± 0.18</v>
       </c>
     </row>
     <row r="7" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
+      <c r="B7" s="22"/>
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
@@ -1103,13 +1103,13 @@
         <f t="shared" ref="F7:G7" si="0">O12 &amp; " " &amp;$M$12&amp; " " &amp; R12</f>
         <v>2.97 ± 0.18</v>
       </c>
-      <c r="G7" s="17" t="str">
+      <c r="G7" s="14" t="str">
         <f t="shared" si="0"/>
         <v>2.75 ± 0.18</v>
       </c>
     </row>
     <row r="8" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
+      <c r="B8" s="22"/>
       <c r="C8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1123,13 +1123,13 @@
         <f t="shared" ref="F8:G8" si="1">O13 &amp; " " &amp;$M$12&amp; " " &amp; R13</f>
         <v>2.95 ± 0.18</v>
       </c>
-      <c r="G8" s="17" t="str">
+      <c r="G8" s="14" t="str">
         <f t="shared" si="1"/>
         <v>2.75 ± 0.16</v>
       </c>
     </row>
     <row r="9" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="4" t="s">
         <v>6</v>
       </c>
@@ -1143,13 +1143,13 @@
         <f t="shared" ref="F9:G9" si="2">O14 &amp; " " &amp;$M$12&amp; " " &amp; R14</f>
         <v>3.02 ± 1.8</v>
       </c>
-      <c r="G9" s="17" t="str">
+      <c r="G9" s="14" t="str">
         <f t="shared" si="2"/>
         <v>2.83 ± 0.17</v>
       </c>
     </row>
     <row r="10" spans="2:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="21" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1165,13 +1165,13 @@
         <f t="shared" ref="F10:G10" si="3">O15 &amp; " " &amp;$M$12&amp; " " &amp; R15</f>
         <v>3.09 ± 0.17</v>
       </c>
-      <c r="G10" s="17" t="str">
+      <c r="G10" s="14" t="str">
         <f t="shared" si="3"/>
         <v>2.87 ± 0.15</v>
       </c>
     </row>
     <row r="11" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B11" s="14"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="4" t="s">
         <v>10</v>
       </c>
@@ -1185,7 +1185,7 @@
         <f t="shared" ref="F11:G11" si="4">O16 &amp; " " &amp;$M$12&amp; " " &amp; R16</f>
         <v>3.04 ± 0.17</v>
       </c>
-      <c r="G11" s="17" t="str">
+      <c r="G11" s="14" t="str">
         <f t="shared" si="4"/>
         <v>2.89 ± 0.15</v>
       </c>
@@ -1203,23 +1203,23 @@
       </c>
     </row>
     <row r="12" spans="2:19" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="18">
+      <c r="D12" s="15">
         <v>-22.611000000000001</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="15">
         <v>11</v>
       </c>
-      <c r="F12" s="18" t="str">
+      <c r="F12" s="15" t="str">
         <f t="shared" ref="F12:G12" si="5">O17 &amp; " " &amp;$M$12&amp; " " &amp; R17</f>
         <v>3.5 ± 0.1</v>
       </c>
-      <c r="G12" s="19" t="str">
+      <c r="G12" s="16" t="str">
         <f t="shared" si="5"/>
         <v>3.26 ± 0.11</v>
       </c>
@@ -1240,6 +1240,10 @@
       </c>
     </row>
     <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <f>SUM(E6:E12)</f>
+        <v>240</v>
+      </c>
       <c r="O13">
         <v>2.95</v>
       </c>
@@ -1533,7 +1537,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFA25DE5-CA98-4D39-ADF0-60F266288A32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="F2:S35"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1782,7 +1786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71655DEB-DBAC-4E1F-819F-E0CBB14B9382}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E2:V62"/>
   <sheetViews>
     <sheetView topLeftCell="F13" workbookViewId="0">
@@ -2500,10 +2504,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AEE9A3E-A58B-4E8E-B5EA-1C6431F52BFB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13:H28"/>
     </sheetView>
   </sheetViews>
@@ -2513,21 +2517,21 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="24"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2535,38 +2539,38 @@
       <c r="B6" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="19">
         <v>2.4605000000000001</v>
       </c>
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="20">
         <v>3.1149</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="20">
         <v>2.8235999999999999</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="24"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="17" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2574,7 +2578,7 @@
       <c r="B10" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="19">
         <v>1.46E-2</v>
       </c>
       <c r="D10" s="7"/>
@@ -2583,7 +2587,7 @@
       <c r="B11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="19">
         <v>2.2700000000000001E-2</v>
       </c>
       <c r="D11" s="7">
@@ -2591,15 +2595,15 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
+      <c r="B13" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="23"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="27"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="7" t="s">
@@ -2641,10 +2645,10 @@
       <c r="B16" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="26">
+      <c r="C16" s="19">
         <v>1.8308</v>
       </c>
-      <c r="D16" s="26">
+      <c r="D16" s="19">
         <v>2.5093000000000001</v>
       </c>
       <c r="E16" s="2"/>
@@ -2656,13 +2660,13 @@
       <c r="B17" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="26">
+      <c r="C17" s="19">
         <v>4.1090999999999998</v>
       </c>
-      <c r="D17" s="26">
+      <c r="D17" s="19">
         <v>4.4283000000000001</v>
       </c>
-      <c r="E17" s="26">
+      <c r="E17" s="19">
         <v>4.5022000000000002</v>
       </c>
       <c r="F17" s="2"/>
@@ -2673,16 +2677,16 @@
       <c r="B18" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="26">
+      <c r="C18" s="19">
         <v>3.4508000000000001</v>
       </c>
-      <c r="D18" s="26">
+      <c r="D18" s="19">
         <v>4.1383999999999999</v>
       </c>
-      <c r="E18" s="26">
+      <c r="E18" s="19">
         <v>2.9769999999999999</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="19">
         <v>4.9272</v>
       </c>
       <c r="G18" s="2"/>
@@ -2692,19 +2696,19 @@
       <c r="B19" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C19" s="26">
+      <c r="C19" s="19">
         <v>3.1465999999999998</v>
       </c>
-      <c r="D19" s="26">
+      <c r="D19" s="19">
         <v>4.2207999999999997</v>
       </c>
-      <c r="E19" s="26">
+      <c r="E19" s="19">
         <v>2.9916</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="19">
         <v>4.5648999999999997</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="19">
         <v>3.0139999999999998</v>
       </c>
       <c r="H19" s="2"/>
@@ -2713,35 +2717,35 @@
       <c r="B20" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="26">
+      <c r="C20" s="19">
         <v>4.8761000000000001</v>
       </c>
-      <c r="D20" s="26">
+      <c r="D20" s="19">
         <v>5.0438000000000001</v>
       </c>
-      <c r="E20" s="26">
+      <c r="E20" s="19">
         <v>4.8564999999999996</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="19">
         <v>2.7393999999999998</v>
       </c>
-      <c r="G20" s="26">
+      <c r="G20" s="19">
         <v>4.8597999999999999</v>
       </c>
-      <c r="H20" s="26">
+      <c r="H20" s="19">
         <v>4.5795000000000003</v>
       </c>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
+      <c r="B21" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="22"/>
-      <c r="D21" s="22"/>
-      <c r="E21" s="22"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="27"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="7" t="s">
@@ -2783,10 +2787,10 @@
       <c r="B24" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="19">
         <v>1.8599999999999998E-2</v>
       </c>
-      <c r="D24" s="26">
+      <c r="D24" s="19">
         <v>2.41E-2</v>
       </c>
       <c r="E24" s="2"/>
@@ -2798,13 +2802,13 @@
       <c r="B25" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="19">
         <v>3.8399999999999997E-2</v>
       </c>
-      <c r="D25" s="26">
+      <c r="D25" s="19">
         <v>3.9899999999999998E-2</v>
       </c>
-      <c r="E25" s="26">
+      <c r="E25" s="19">
         <v>3.9300000000000002E-2</v>
       </c>
       <c r="F25" s="2"/>
@@ -2815,16 +2819,16 @@
       <c r="B26" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="19">
         <v>2.58E-2</v>
       </c>
-      <c r="D26" s="26">
+      <c r="D26" s="19">
         <v>3.0599999999999999E-2</v>
       </c>
-      <c r="E26" s="26">
+      <c r="E26" s="19">
         <v>2.0299999999999999E-2</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="19">
         <v>3.9300000000000002E-2</v>
       </c>
       <c r="G26" s="2"/>
@@ -2834,19 +2838,19 @@
       <c r="B27" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="19">
         <v>1.84E-2</v>
       </c>
-      <c r="D27" s="26">
+      <c r="D27" s="19">
         <v>2.64E-2</v>
       </c>
-      <c r="E27" s="26">
+      <c r="E27" s="19">
         <v>1.7600000000000001E-2</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="19">
         <v>3.61E-2</v>
       </c>
-      <c r="G27" s="26">
+      <c r="G27" s="19">
         <v>1.7899999999999999E-2</v>
       </c>
       <c r="H27" s="2"/>
@@ -2855,22 +2859,22 @@
       <c r="B28" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="19">
         <v>4.9500000000000002E-2</v>
       </c>
-      <c r="D28" s="26">
+      <c r="D28" s="19">
         <v>5.1499999999999997E-2</v>
       </c>
-      <c r="E28" s="26">
+      <c r="E28" s="19">
         <v>4.2900000000000001E-2</v>
       </c>
-      <c r="F28" s="26">
+      <c r="F28" s="19">
         <v>2.3E-2</v>
       </c>
-      <c r="G28" s="26">
+      <c r="G28" s="19">
         <v>4.0099999999999997E-2</v>
       </c>
-      <c r="H28" s="26">
+      <c r="H28" s="19">
         <v>4.24E-2</v>
       </c>
     </row>
@@ -2887,7 +2891,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CE33CB1-D7F9-488F-97A3-3C3D8E907569}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E3:P32"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>